<commit_message>
Updated All Errors In The Program
</commit_message>
<xml_diff>
--- a/ProjectB/src/test/resources/ProjectTeamB.xlsx
+++ b/ProjectB/src/test/resources/ProjectTeamB.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avina\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avina\git\repository\ProjectB\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B33158-3FD9-40FD-AC7C-E52146B2C39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5112F01E-DA4F-43A6-A87F-91AFA0A1747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{64DA74A5-921D-4564-952D-397A94D753FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CO_Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>